<commit_message>
Ajout du folder dans le guide d'implémentation 83a1848f064726c23fceeb0e0807bdbf6aac23e5
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-DocumentEntry.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-DocumentEntry.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-06T13:57:20+00:00</t>
+    <t>2025-05-19T16:11:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -279,16 +279,20 @@
     <t>DocumentEntry.mimeType</t>
   </si>
   <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Cette métadonnée représente le type de contenu du document, défini par le standard MIME.</t>
+  </si>
+  <si>
+    <t>DocumentEntry.availabilityStatus</t>
+  </si>
+  <si>
     <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
-    <t>Cette métadonnée représente le type de contenu du document, défini par le standard MIME.</t>
-  </si>
-  <si>
-    <t>DocumentEntry.availabilityStatus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cette métadonnée représente la pertinence de la version de la fiche d'un document. </t>
   </si>
   <si>
@@ -305,10 +309,6 @@
   </si>
   <si>
     <t>DocumentEntry.hash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
   </si>
   <si>
     <t>Cette métadonnée contient le résultat du hachage du document déposé</t>
@@ -1506,13 +1506,13 @@
         <v>73</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1539,11 +1539,11 @@
         <v>73</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y6" s="2"/>
       <c r="Z6" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>73</v>
@@ -1576,15 +1576,15 @@
         <v>73</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -1607,7 +1607,7 @@
         <v>73</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L7" t="s" s="2">
         <v>97</v>
@@ -1664,7 +1664,7 @@
         <v>73</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>79</v>
@@ -1813,7 +1813,7 @@
         <v>73</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L9" t="s" s="2">
         <v>102</v>
@@ -2637,7 +2637,7 @@
         <v>73</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L17" t="s" s="2">
         <v>126</v>
@@ -2740,7 +2740,7 @@
         <v>73</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L18" t="s" s="2">
         <v>128</v>
@@ -2843,7 +2843,7 @@
         <v>73</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L19" t="s" s="2">
         <v>130</v>
@@ -3152,7 +3152,7 @@
         <v>73</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L22" t="s" s="2">
         <v>138</v>
@@ -3185,7 +3185,7 @@
         <v>73</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y22" s="2"/>
       <c r="Z22" t="s" s="2">
@@ -3253,7 +3253,7 @@
         <v>73</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L23" t="s" s="2">
         <v>144</v>
@@ -3286,7 +3286,7 @@
         <v>73</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y23" s="2"/>
       <c r="Z23" t="s" s="2">
@@ -3457,7 +3457,7 @@
         <v>73</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L25" t="s" s="2">
         <v>152</v>
@@ -3490,7 +3490,7 @@
         <v>73</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y25" s="2"/>
       <c r="Z25" t="s" s="2">
@@ -3558,7 +3558,7 @@
         <v>73</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L26" t="s" s="2">
         <v>156</v>
@@ -3591,7 +3591,7 @@
         <v>73</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y26" s="2"/>
       <c r="Z26" t="s" s="2">
@@ -3659,7 +3659,7 @@
         <v>73</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L27" t="s" s="2">
         <v>160</v>
@@ -3692,7 +3692,7 @@
         <v>73</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y27" s="2"/>
       <c r="Z27" t="s" s="2">
@@ -3760,7 +3760,7 @@
         <v>73</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L28" t="s" s="2">
         <v>164</v>
@@ -3793,7 +3793,7 @@
         <v>73</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y28" s="2"/>
       <c r="Z28" t="s" s="2">
@@ -3861,7 +3861,7 @@
         <v>73</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L29" t="s" s="2">
         <v>168</v>
@@ -4479,7 +4479,7 @@
         <v>73</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L35" t="s" s="2">
         <v>182</v>
@@ -4512,7 +4512,7 @@
         <v>73</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Y35" s="2"/>
       <c r="Z35" t="s" s="2">

</xml_diff>